<commit_message>
450 question bank array problme 6 solved
</commit_message>
<xml_diff>
--- a/450-Questions-List/DSA-Questions.xlsx
+++ b/450-Questions-List/DSA-Questions.xlsx
@@ -1879,7 +1879,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2007,8 +2007,8 @@
       <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
+      <c r="C11" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D11" s="7">
         <v>6</v>

</xml_diff>

<commit_message>
450 questions array section problem 8 solved
</commit_message>
<xml_diff>
--- a/450-Questions-List/DSA-Questions.xlsx
+++ b/450-Questions-List/DSA-Questions.xlsx
@@ -1879,7 +1879,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2035,8 +2035,8 @@
       <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>4</v>
+      <c r="C13" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D13" s="7">
         <v>8</v>

</xml_diff>

<commit_message>
450 questions in array problem 9 completed
</commit_message>
<xml_diff>
--- a/450-Questions-List/DSA-Questions.xlsx
+++ b/450-Questions-List/DSA-Questions.xlsx
@@ -1879,7 +1879,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2049,8 +2049,8 @@
       <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>4</v>
+      <c r="C14" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D14" s="7">
         <v>9</v>

</xml_diff>

<commit_message>
450 questions Array section problem 10 solved
</commit_message>
<xml_diff>
--- a/450-Questions-List/DSA-Questions.xlsx
+++ b/450-Questions-List/DSA-Questions.xlsx
@@ -1879,7 +1879,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2063,8 +2063,8 @@
       <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>4</v>
+      <c r="C15" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D15" s="7">
         <v>10</v>

</xml_diff>

<commit_message>
450 questions array section problem 13 solved
</commit_message>
<xml_diff>
--- a/450-Questions-List/DSA-Questions.xlsx
+++ b/450-Questions-List/DSA-Questions.xlsx
@@ -1879,7 +1879,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2105,8 +2105,8 @@
       <c r="B18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>4</v>
+      <c r="C18" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D18" s="7">
         <v>13</v>

</xml_diff>

<commit_message>
450 questions array section problem14 completed
</commit_message>
<xml_diff>
--- a/450-Questions-List/DSA-Questions.xlsx
+++ b/450-Questions-List/DSA-Questions.xlsx
@@ -1879,7 +1879,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2119,8 +2119,8 @@
       <c r="B19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>4</v>
+      <c r="C19" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D19" s="7">
         <v>14</v>

</xml_diff>

<commit_message>
450 questions => Array Problem 11 solved
</commit_message>
<xml_diff>
--- a/450-Questions-List/DSA-Questions.xlsx
+++ b/450-Questions-List/DSA-Questions.xlsx
@@ -1879,7 +1879,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2077,8 +2077,8 @@
       <c r="B16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>4</v>
+      <c r="C16" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D16" s="7">
         <v>11</v>

</xml_diff>

<commit_message>
450 questions => Array problem 12 solved
</commit_message>
<xml_diff>
--- a/450-Questions-List/DSA-Questions.xlsx
+++ b/450-Questions-List/DSA-Questions.xlsx
@@ -1879,7 +1879,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1890,7 +1890,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2091,8 +2091,8 @@
       <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>4</v>
+      <c r="C17" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D17" s="7">
         <v>12</v>

</xml_diff>

<commit_message>
Git ignore file added, in order to ignore the executable file of the code.
</commit_message>
<xml_diff>
--- a/450-Questions-List/DSA-Questions.xlsx
+++ b/450-Questions-List/DSA-Questions.xlsx
@@ -1879,7 +1879,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2133,8 +2133,8 @@
       <c r="B20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>4</v>
+      <c r="C20" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D20" s="7">
         <v>15</v>
@@ -2147,8 +2147,8 @@
       <c r="B21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>4</v>
+      <c r="C21" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D21" s="7">
         <v>16</v>
@@ -2161,8 +2161,8 @@
       <c r="B22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>4</v>
+      <c r="C22" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D22" s="7">
         <v>17</v>
@@ -2603,8 +2603,8 @@
       <c r="B56" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>4</v>
+      <c r="C56" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D56" s="7">
         <v>47</v>
@@ -2617,8 +2617,8 @@
       <c r="B57" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>4</v>
+      <c r="C57" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D57" s="7">
         <v>48</v>
@@ -2631,8 +2631,8 @@
       <c r="B58" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>4</v>
+      <c r="C58" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D58" s="7">
         <v>49</v>
@@ -2659,8 +2659,8 @@
       <c r="B60" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>4</v>
+      <c r="C60" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D60" s="7">
         <v>51</v>
@@ -2673,8 +2673,8 @@
       <c r="B61" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>4</v>
+      <c r="C61" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D61" s="7">
         <v>52</v>

</xml_diff>

<commit_message>
450 Questions => String ==> Problem 57 solved.
</commit_message>
<xml_diff>
--- a/450-Questions-List/DSA-Questions.xlsx
+++ b/450-Questions-List/DSA-Questions.xlsx
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="B58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2175,8 +2175,8 @@
       <c r="B23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>4</v>
+      <c r="C23" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D23" s="7">
         <v>18</v>
@@ -2189,8 +2189,8 @@
       <c r="B24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>4</v>
+      <c r="C24" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D24" s="7">
         <v>19</v>
@@ -2217,8 +2217,8 @@
       <c r="B26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>4</v>
+      <c r="C26" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D26" s="7">
         <v>21</v>
@@ -2231,8 +2231,8 @@
       <c r="B27" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>4</v>
+      <c r="C27" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D27" s="7">
         <v>22</v>
@@ -2245,8 +2245,8 @@
       <c r="B28" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>4</v>
+      <c r="C28" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D28" s="7">
         <v>23</v>
@@ -2259,8 +2259,8 @@
       <c r="B29" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>4</v>
+      <c r="C29" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D29" s="7">
         <v>24</v>
@@ -2687,8 +2687,8 @@
       <c r="B62" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>4</v>
+      <c r="C62" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D62" s="7">
         <v>53</v>
@@ -2701,8 +2701,8 @@
       <c r="B63" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>4</v>
+      <c r="C63" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D63" s="7">
         <v>54</v>
@@ -2715,8 +2715,8 @@
       <c r="B64" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C64" s="4" t="s">
-        <v>4</v>
+      <c r="C64" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D64" s="7">
         <v>55</v>
@@ -2729,8 +2729,8 @@
       <c r="B65" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>4</v>
+      <c r="C65" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D65" s="7">
         <v>56</v>
@@ -2743,8 +2743,8 @@
       <c r="B66" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>4</v>
+      <c r="C66" s="11" t="s">
+        <v>466</v>
       </c>
       <c r="D66" s="7">
         <v>57</v>

</xml_diff>